<commit_message>
Sent for groupmates to check
</commit_message>
<xml_diff>
--- a/data/warehouse_cost.xlsx
+++ b/data/warehouse_cost.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alqer\Desktop\uni\s2\supply-chain-management\project\facility-location-problem\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\uni\s2\supply-chain-management\project\facility-location-problem\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF14F4D5-70F3-4725-91F5-77E046477796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -126,7 +125,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -205,7 +204,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_mesafe cetveli-2004" xfId="1" xr:uid="{0FEA901A-150D-4393-B615-C7F07553983C}"/>
+    <cellStyle name="Normal_mesafe cetveli-2004" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -482,11 +481,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,240 +506,240 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>21628</v>
+      <c r="B2">
+        <v>733.15254237288138</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
-        <v>30553</v>
+      <c r="B3">
+        <v>1035.6949152542372</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
-        <v>37764</v>
+      <c r="B4">
+        <v>1280.1355932203389</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
-        <v>13478</v>
+      <c r="B5">
+        <v>456.88135593220341</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
-        <v>16647</v>
+      <c r="B6">
+        <v>564.30508474576266</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
-        <v>19433</v>
+      <c r="B7">
+        <v>658.74576271186436</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
-        <v>40000</v>
+      <c r="B8">
+        <v>1355.9322033898304</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
-        <v>10500</v>
+      <c r="B9">
+        <v>355.93220338983053</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
-        <v>13500</v>
+      <c r="B10">
+        <v>457.62711864406782</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
-        <v>22666</v>
+      <c r="B11">
+        <v>768.33898305084745</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
-        <v>18012</v>
+      <c r="B12">
+        <v>610.57627118644064</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
-        <v>18000</v>
+      <c r="B13">
+        <v>610.16949152542372</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
-        <v>28333</v>
+      <c r="B14">
+        <v>960.4406779661017</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
-        <v>46131</v>
+      <c r="B15">
+        <v>1563.7627118644068</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
-        <v>30120</v>
+      <c r="B16">
+        <v>1021.0169491525423</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2">
-        <v>35000</v>
+      <c r="B17">
+        <v>1186.4406779661017</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
-        <v>22500</v>
+      <c r="B18">
+        <v>762.71186440677968</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2">
-        <v>17666</v>
+      <c r="B19">
+        <v>598.84745762711862</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2">
-        <v>19000</v>
+      <c r="B20">
+        <v>644.06779661016947</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2">
-        <v>18000</v>
+      <c r="B21">
+        <v>610.16949152542372</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2">
-        <v>25000</v>
+      <c r="B22">
+        <v>847.45762711864404</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2">
-        <v>55000</v>
+      <c r="B23">
+        <v>1864.406779661017</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2">
-        <v>16000</v>
+      <c r="B24">
+        <v>542.37288135593224</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2">
-        <v>14000</v>
+      <c r="B25">
+        <v>474.57627118644069</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2">
-        <v>20000</v>
+      <c r="B26">
+        <v>677.96610169491521</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="2">
-        <v>13171</v>
+      <c r="B27">
+        <v>446.47457627118644</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="2">
-        <v>25000</v>
+      <c r="B28">
+        <v>847.45762711864404</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="2">
-        <v>30000</v>
+      <c r="B29">
+        <v>1016.9491525423729</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="2">
-        <v>11000</v>
+      <c r="B30">
+        <v>372.88135593220341</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="2">
-        <v>10000</v>
+      <c r="B31">
+        <v>338.9830508474576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>